<commit_message>
Updating Self Learning TC02 Version 2.0
</commit_message>
<xml_diff>
--- a/Self_Learning_Testcases_and_Results/Self Learning TC02.xlsx
+++ b/Self_Learning_Testcases_and_Results/Self Learning TC02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Class12Capstone\Self_Learning_Testcases_and_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19EA5FF8-9D30-47FF-B349-4DC0920BFDE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F423D9BE-0E44-4485-B013-9C21F161FE2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D5087028-81F7-4AD3-873A-FC8287C14187}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{54D4E008-6D52-4BC6-8B2C-DBF630EDEB50}"/>
   </bookViews>
   <sheets>
     <sheet name="Self Learning TC2" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">AC4 Nmap tool should work properly and allow you to view a specific targets IP address, as well as show you any open ports that hackers may be able to access from that address or URL. </t>
   </si>
@@ -47,7 +47,7 @@
     <t>Your internet connection is working properly</t>
   </si>
   <si>
-    <t>You know the URL for the website you wish to scan</t>
+    <t>You know the IP Address for the website you wish to scan</t>
   </si>
   <si>
     <t xml:space="preserve"> Test Scenario</t>
@@ -65,7 +65,7 @@
     <t>Pass/Fail</t>
   </si>
   <si>
-    <t>AC4TC2: Ensure you're able to find the IP Address from the Nmap desktop application</t>
+    <t>AC4TC2: Ensure you're able to scan the website fully from the Nmap desktop application</t>
   </si>
   <si>
     <t>1.Initialize the "Zenmap" application from your desktop</t>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nmap should populate detailed information on the website you scanned showing you the IP address and the amount of ports that are actively open. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Scroll down the information to find the active open ports. Take note of which ports are open as these may be vulnerable to attack. There should also be detailed information on a tracerout showing you where the packet information travels from and how fast it takes to do so. </t>
   </si>
 </sst>
 </file>
@@ -568,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754DA748-2522-4DDE-B11E-A37A2CA9A529}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD8A6BC-C05F-4B15-9F95-12706991F640}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,8 +667,10 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="11"/>
+    <row r="14" spans="1:5" ht="102" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" s="11"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>

</xml_diff>